<commit_message>
Make Guardar/Verificar/Finalizar buttons smaller on mobile: 38px height, 13px font
</commit_message>
<xml_diff>
--- a/uploads/1/ota.xlsx
+++ b/uploads/1/ota.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app_auditorias\uploads\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AAE931-A0AE-4456-9FA6-E65B07D45953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C821C264-BB9B-4E00-B639-012631EEEB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB4C2080-33BF-4064-94D0-2BB3462F5794}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>